<commit_message>
report with inv, chart, wiring diags and dodgy conc
</commit_message>
<xml_diff>
--- a/drone gantt chart.xlsx
+++ b/drone gantt chart.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jemma\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Receive Arduino 101</t>
   </si>
@@ -123,13 +118,16 @@
   </si>
   <si>
     <t>Tasks</t>
+  </si>
+  <si>
+    <t>Gantt Chart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +138,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -306,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -322,6 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -636,10 +643,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AO24"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AO24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD13" sqref="AD13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,6 +658,11 @@
     <col min="2" max="43" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:41" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -1774,6 +1789,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>